<commit_message>
Added Student Marks and Student Progress Report
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/App Tasks Pending.xlsx
+++ b/src/main/resources/templates/App Tasks Pending.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EC03E0-1616-4EE3-9A4B-42674959A474}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F1AA6E-23D3-4BB3-A04A-FC5932735B73}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
   <si>
     <t>spring security</t>
   </si>
@@ -558,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,10 +955,16 @@
       <c r="A53" t="s">
         <v>57</v>
       </c>
+      <c r="B53" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>59</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>